<commit_message>
update csv files and sources for upstream and industrial sectors, latest version of Reference and Net Zero notebooks, latest version CSV Editor and Results Viewer
</commit_message>
<xml_diff>
--- a/csv/model/FIC/formula_FIC_QC.xlsx
+++ b/csv/model/FIC/formula_FIC_QC.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CIMS\dev\cims-models\csv\model\FIC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{745552F9-BAF1-4D63-9E2E-F6B15F175D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F645C2DD-9C7C-47F1-933E-3AD969E5924A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{02DD8B11-9E2F-41AB-9FC3-7D0099BED657}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{21759449-8EA4-4D11-9B33-D188AAA961B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcCompleted="0" calcOnSave="0"/>
+  <calcPr calcId="191029" iterate="1" calcCompleted="0" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -653,7 +653,7 @@
     <t>BPST NG 30 MW CCS</t>
   </si>
   <si>
-    <t>Coal steam turbine CCS</t>
+    <t>Coal CCS</t>
   </si>
   <si>
     <t>CIMS.CAN.QC.Iron and Steel.HVAC.Space Heating</t>
@@ -1936,21 +1936,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A978B406-177F-4D37-9F46-D772FF3F3D88}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5EDBD4C-0958-47E9-86CE-23FB2F424340}">
   <dimension ref="A1:X386"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:X386"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -2162,7 +2162,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>-400000</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -2300,7 +2300,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -2438,7 +2438,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -2507,7 +2507,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>15668162.1880998</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -2714,7 +2714,7 @@
         <v>855.18234165067202</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -2852,7 +2852,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>-30000000</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -2990,7 +2990,7 @@
         <v>400000000</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -3059,7 +3059,7 @@
         <v>-500000000</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>-1800000000</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -3197,7 +3197,7 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -3266,7 +3266,7 @@
         <v>-13000000</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>57</v>
       </c>
@@ -3335,7 +3335,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>57</v>
       </c>
@@ -3404,7 +3404,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>57</v>
       </c>
@@ -3473,7 +3473,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -3542,7 +3542,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>57</v>
       </c>
@@ -3611,7 +3611,7 @@
         <v>400000000</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>57</v>
       </c>
@@ -3680,7 +3680,7 @@
         <v>-1800000000</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -3749,7 +3749,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>61</v>
       </c>
@@ -3818,7 +3818,7 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>61</v>
       </c>
@@ -3887,7 +3887,7 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -3956,7 +3956,7 @@
         <v>39692.677543186102</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>64</v>
       </c>
@@ -4025,7 +4025,7 @@
         <v>28968.690978886701</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>69</v>
       </c>
@@ -4094,7 +4094,7 @@
         <v>233977.88867562299</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>69</v>
       </c>
@@ -4163,7 +4163,7 @@
         <v>220607.723608445</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>69</v>
       </c>
@@ -4232,7 +4232,7 @@
         <v>5813932.7159308996</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>69</v>
       </c>
@@ -4301,7 +4301,7 @@
         <v>3924004.1746641002</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>75</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>5412929.4695297498</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>75</v>
       </c>
@@ -4439,7 +4439,7 @@
         <v>4786577.7229078701</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>75</v>
       </c>
@@ -4508,7 +4508,7 @@
         <v>6892560.5816218797</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>75</v>
       </c>
@@ -4577,7 +4577,7 @@
         <v>8469605.0500095896</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>75</v>
       </c>
@@ -4646,7 +4646,7 @@
         <v>5967163.5060268696</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>75</v>
       </c>
@@ -4715,7 +4715,7 @@
         <v>6916183.6133013396</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>83</v>
       </c>
@@ -4784,7 +4784,7 @@
         <v>8874447.0633397307</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>83</v>
       </c>
@@ -4853,7 +4853,7 @@
         <v>4437223.5316698598</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>83</v>
       </c>
@@ -4922,7 +4922,7 @@
         <v>8851884.9097888693</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>83</v>
       </c>
@@ -4991,7 +4991,7 @@
         <v>4425942.45489443</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>89</v>
       </c>
@@ -5060,7 +5060,7 @@
         <v>392400.41746641003</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>89</v>
       </c>
@@ -5129,7 +5129,7 @@
         <v>394106.50623800303</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>89</v>
       </c>
@@ -5198,7 +5198,7 @@
         <v>392400.41746641003</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>94</v>
       </c>
@@ -5267,7 +5267,7 @@
         <v>174647781.19001901</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>94</v>
       </c>
@@ -5336,7 +5336,7 @@
         <v>175483416.506717</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>98</v>
       </c>
@@ -5405,7 +5405,7 @@
         <v>14239922.159309</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>98</v>
       </c>
@@ -5474,7 +5474,7 @@
         <v>8237971.4971209196</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>102</v>
       </c>
@@ -5543,7 +5543,7 @@
         <v>14239922.159309</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>102</v>
       </c>
@@ -5612,7 +5612,7 @@
         <v>14258027.591170801</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>105</v>
       </c>
@@ -5681,7 +5681,7 @@
         <v>14239922.159309</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>105</v>
       </c>
@@ -5750,7 +5750,7 @@
         <v>14258027.591170801</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>105</v>
       </c>
@@ -5819,7 +5819,7 @@
         <v>5953901.6314779203</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>105</v>
       </c>
@@ -5888,7 +5888,7 @@
         <v>6032242.4424184198</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>110</v>
       </c>
@@ -5957,7 +5957,7 @@
         <v>1295234.7408829101</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>110</v>
       </c>
@@ -6026,7 +6026,7 @@
         <v>1278522.0345489399</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>110</v>
       </c>
@@ -6095,7 +6095,7 @@
         <v>4014047.2152495198</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>110</v>
       </c>
@@ -6164,7 +6164,7 @@
         <v>3295422.03919385</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>116</v>
       </c>
@@ -6233,7 +6233,7 @@
         <v>3665653.58925144</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>116</v>
       </c>
@@ -6302,7 +6302,7 @@
         <v>3689051.3781189998</v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>116</v>
       </c>
@@ -6371,7 +6371,7 @@
         <v>2084213.7523992299</v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>116</v>
       </c>
@@ -6440,7 +6440,7 @@
         <v>2068963.4078694801</v>
       </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>122</v>
       </c>
@@ -6509,7 +6509,7 @@
         <v>21935427.063339699</v>
       </c>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>122</v>
       </c>
@@ -6578,7 +6578,7 @@
         <v>24128969.769673701</v>
       </c>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>125</v>
       </c>
@@ -6647,7 +6647,7 @@
         <v>855.18234165067202</v>
       </c>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>126</v>
       </c>
@@ -6716,7 +6716,7 @@
         <v>1227368.459</v>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>126</v>
       </c>
@@ -6785,7 +6785,7 @@
         <v>1227368.459</v>
       </c>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>126</v>
       </c>
@@ -6854,7 +6854,7 @@
         <v>1227368.459</v>
       </c>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>132</v>
       </c>
@@ -6923,7 +6923,7 @@
         <v>2007483.341</v>
       </c>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>135</v>
       </c>
@@ -6992,7 +6992,7 @@
         <v>855.18234165067202</v>
       </c>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>136</v>
       </c>
@@ -7061,7 +7061,7 @@
         <v>226499393.31549901</v>
       </c>
     </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>140</v>
       </c>
@@ -7130,7 +7130,7 @@
         <v>350000000</v>
       </c>
     </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>140</v>
       </c>
@@ -7199,7 +7199,7 @@
         <v>700000000</v>
       </c>
     </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>140</v>
       </c>
@@ -7268,7 +7268,7 @@
         <v>700000000</v>
       </c>
     </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>140</v>
       </c>
@@ -7337,7 +7337,7 @@
         <v>200000000</v>
       </c>
     </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>140</v>
       </c>
@@ -7406,7 +7406,7 @@
         <v>200000000</v>
       </c>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>140</v>
       </c>
@@ -7475,7 +7475,7 @@
         <v>700000000</v>
       </c>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>140</v>
       </c>
@@ -7544,7 +7544,7 @@
         <v>700000000</v>
       </c>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>140</v>
       </c>
@@ -7613,7 +7613,7 @@
         <v>200000000</v>
       </c>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>150</v>
       </c>
@@ -7682,7 +7682,7 @@
         <v>645093208.90306103</v>
       </c>
     </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>150</v>
       </c>
@@ -7751,7 +7751,7 @@
         <v>836231936.95608401</v>
       </c>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>150</v>
       </c>
@@ -7820,7 +7820,7 @@
         <v>836231936.95608401</v>
       </c>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>155</v>
       </c>
@@ -7889,7 +7889,7 @@
         <v>344049711.411708</v>
       </c>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>155</v>
       </c>
@@ -7958,7 +7958,7 @@
         <v>535188439.77015299</v>
       </c>
     </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>159</v>
       </c>
@@ -8027,7 +8027,7 @@
         <v>344049711.411708</v>
       </c>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>159</v>
       </c>
@@ -8096,7 +8096,7 @@
         <v>305821965.49568099</v>
       </c>
     </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>163</v>
       </c>
@@ -8165,7 +8165,7 @@
         <v>140168400.877639</v>
       </c>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>166</v>
       </c>
@@ -8234,7 +8234,7 @@
         <v>573416185.07533598</v>
       </c>
     </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>169</v>
       </c>
@@ -8303,7 +8303,7 @@
         <v>183493179.23632401</v>
       </c>
     </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>172</v>
       </c>
@@ -8372,7 +8372,7 @@
         <v>183493179.23632401</v>
       </c>
     </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>175</v>
       </c>
@@ -8441,7 +8441,7 @@
         <v>382277456.71688998</v>
       </c>
     </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>178</v>
       </c>
@@ -8510,7 +8510,7 @@
         <v>645093208.90306103</v>
       </c>
     </row>
-    <row r="97" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>178</v>
       </c>
@@ -8579,7 +8579,7 @@
         <v>621200867.31765795</v>
       </c>
     </row>
-    <row r="98" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>182</v>
       </c>
@@ -8648,7 +8648,7 @@
         <v>382277456.71688998</v>
       </c>
     </row>
-    <row r="99" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>185</v>
       </c>
@@ -8717,7 +8717,7 @@
         <v>382277456.71688998</v>
       </c>
     </row>
-    <row r="100" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>188</v>
       </c>
@@ -8786,7 +8786,7 @@
         <v>645093208.90306103</v>
       </c>
     </row>
-    <row r="101" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>188</v>
       </c>
@@ -8855,7 +8855,7 @@
         <v>573416185.68618</v>
       </c>
     </row>
-    <row r="102" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>192</v>
       </c>
@@ -8924,7 +8924,7 @@
         <v>382277456.71688998</v>
       </c>
     </row>
-    <row r="103" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>195</v>
       </c>
@@ -8993,7 +8993,7 @@
         <v>1274258187.63099</v>
       </c>
     </row>
-    <row r="104" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>198</v>
       </c>
@@ -9062,7 +9062,7 @@
         <v>-28670809.284309</v>
       </c>
     </row>
-    <row r="105" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>201</v>
       </c>
@@ -9131,7 +9131,7 @@
         <v>10016749.390000001</v>
       </c>
     </row>
-    <row r="106" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>201</v>
       </c>
@@ -9200,7 +9200,7 @@
         <v>15668162.189999999</v>
       </c>
     </row>
-    <row r="107" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>201</v>
       </c>
@@ -9269,7 +9269,7 @@
         <v>15668162.189999999</v>
       </c>
     </row>
-    <row r="108" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>201</v>
       </c>
@@ -9338,7 +9338,7 @@
         <v>15668162.189999999</v>
       </c>
     </row>
-    <row r="109" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>201</v>
       </c>
@@ -9407,7 +9407,7 @@
         <v>15668162.189999999</v>
       </c>
     </row>
-    <row r="110" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>206</v>
       </c>
@@ -9476,7 +9476,7 @@
         <v>610844.52975047997</v>
       </c>
     </row>
-    <row r="111" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>209</v>
       </c>
@@ -9545,7 +9545,7 @@
         <v>855.18234165067202</v>
       </c>
     </row>
-    <row r="112" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>210</v>
       </c>
@@ -9614,7 +9614,7 @@
         <v>114005.127629558</v>
       </c>
     </row>
-    <row r="113" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>210</v>
       </c>
@@ -9683,7 +9683,7 @@
         <v>114005.127629558</v>
       </c>
     </row>
-    <row r="114" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>214</v>
       </c>
@@ -9752,7 +9752,7 @@
         <v>37766.684740882898</v>
       </c>
     </row>
-    <row r="115" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>214</v>
       </c>
@@ -9821,7 +9821,7 @@
         <v>73501.089731286003</v>
       </c>
     </row>
-    <row r="116" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>214</v>
       </c>
@@ -9890,7 +9890,7 @@
         <v>73501.089731286003</v>
       </c>
     </row>
-    <row r="117" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>219</v>
       </c>
@@ -9959,7 +9959,7 @@
         <v>126499.793666026</v>
       </c>
     </row>
-    <row r="118" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>219</v>
       </c>
@@ -10028,7 +10028,7 @@
         <v>142625.90599808001</v>
       </c>
     </row>
-    <row r="119" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>219</v>
       </c>
@@ -10097,7 +10097,7 @@
         <v>99623.856046065193</v>
       </c>
     </row>
-    <row r="120" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>224</v>
       </c>
@@ -10166,7 +10166,7 @@
         <v>479652.83925143903</v>
       </c>
     </row>
-    <row r="121" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>224</v>
       </c>
@@ -10235,7 +10235,7 @@
         <v>528764.55619001901</v>
       </c>
     </row>
-    <row r="122" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>224</v>
       </c>
@@ -10304,7 +10304,7 @@
         <v>397800.89395393402</v>
       </c>
     </row>
-    <row r="123" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>226</v>
       </c>
@@ -10373,7 +10373,7 @@
         <v>65152.066698656403</v>
       </c>
     </row>
-    <row r="124" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>226</v>
       </c>
@@ -10442,7 +10442,7 @@
         <v>66984.600287907801</v>
       </c>
     </row>
-    <row r="125" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>229</v>
       </c>
@@ -10511,7 +10511,7 @@
         <v>393930.58301343501</v>
       </c>
     </row>
-    <row r="126" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>229</v>
       </c>
@@ -10580,7 +10580,7 @@
         <v>397595.65019193798</v>
       </c>
     </row>
-    <row r="127" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>230</v>
       </c>
@@ -10649,7 +10649,7 @@
         <v>138453.41026871401</v>
       </c>
     </row>
-    <row r="128" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>232</v>
       </c>
@@ -10718,7 +10718,7 @@
         <v>687135.95729366597</v>
       </c>
     </row>
-    <row r="129" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>233</v>
       </c>
@@ -10787,7 +10787,7 @@
         <v>138453.41026871401</v>
       </c>
     </row>
-    <row r="130" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>235</v>
       </c>
@@ -10856,7 +10856,7 @@
         <v>687135.95729366597</v>
       </c>
     </row>
-    <row r="131" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>236</v>
       </c>
@@ -10925,7 +10925,7 @@
         <v>1171.44098848368</v>
       </c>
     </row>
-    <row r="132" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>239</v>
       </c>
@@ -10994,7 +10994,7 @@
         <v>3911.90945297504</v>
       </c>
     </row>
-    <row r="133" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>242</v>
       </c>
@@ -11063,7 +11063,7 @@
         <v>16256.051180422201</v>
       </c>
     </row>
-    <row r="134" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>245</v>
       </c>
@@ -11132,7 +11132,7 @@
         <v>30828.321631477898</v>
       </c>
     </row>
-    <row r="135" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>248</v>
       </c>
@@ -11201,7 +11201,7 @@
         <v>139242.926823416</v>
       </c>
     </row>
-    <row r="136" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>251</v>
       </c>
@@ -11270,7 +11270,7 @@
         <v>440179.03952015302</v>
       </c>
     </row>
-    <row r="137" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>254</v>
       </c>
@@ -11339,7 +11339,7 @@
         <v>15668162.1880998</v>
       </c>
     </row>
-    <row r="138" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>256</v>
       </c>
@@ -11408,7 +11408,7 @@
         <v>855.18234165067202</v>
       </c>
     </row>
-    <row r="139" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>257</v>
       </c>
@@ -11477,7 +11477,7 @@
         <v>335108748.253618</v>
       </c>
     </row>
-    <row r="140" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>257</v>
       </c>
@@ -11546,7 +11546,7 @@
         <v>340241705.00061399</v>
       </c>
     </row>
-    <row r="141" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>262</v>
       </c>
@@ -11615,7 +11615,7 @@
         <v>4507308.9986948101</v>
       </c>
     </row>
-    <row r="142" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>262</v>
       </c>
@@ -11684,7 +11684,7 @@
         <v>6131520.0229174597</v>
       </c>
     </row>
-    <row r="143" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>266</v>
       </c>
@@ -11753,7 +11753,7 @@
         <v>218376768.33616099</v>
       </c>
     </row>
-    <row r="144" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>266</v>
       </c>
@@ -11822,7 +11822,7 @@
         <v>240214445.17466399</v>
       </c>
     </row>
-    <row r="145" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>270</v>
       </c>
@@ -11891,7 +11891,7 @@
         <v>168464079.84644899</v>
       </c>
     </row>
-    <row r="146" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>273</v>
       </c>
@@ -11960,7 +11960,7 @@
         <v>1228383915.54702</v>
       </c>
     </row>
-    <row r="147" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>276</v>
       </c>
@@ -12029,7 +12029,7 @@
         <v>1228383915.54702</v>
       </c>
     </row>
-    <row r="148" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>278</v>
       </c>
@@ -12098,7 +12098,7 @@
         <v>1228383915.54702</v>
       </c>
     </row>
-    <row r="149" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>280</v>
       </c>
@@ -12167,7 +12167,7 @@
         <v>24476702.058733199</v>
       </c>
     </row>
-    <row r="150" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>280</v>
       </c>
@@ -12236,7 +12236,7 @@
         <v>24476702.058733199</v>
       </c>
     </row>
-    <row r="151" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>284</v>
       </c>
@@ -12305,7 +12305,7 @@
         <v>12534529.750479801</v>
       </c>
     </row>
-    <row r="152" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>284</v>
       </c>
@@ -12374,7 +12374,7 @@
         <v>13579073.896353099</v>
       </c>
     </row>
-    <row r="153" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>284</v>
       </c>
@@ -12443,7 +12443,7 @@
         <v>15668162.1880998</v>
       </c>
     </row>
-    <row r="154" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>284</v>
       </c>
@@ -12512,7 +12512,7 @@
         <v>4317040.5920000002</v>
       </c>
     </row>
-    <row r="155" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>284</v>
       </c>
@@ -12581,7 +12581,7 @@
         <v>10967713.531669799</v>
       </c>
     </row>
-    <row r="156" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>284</v>
       </c>
@@ -12650,7 +12650,7 @@
         <v>26322512.476007599</v>
       </c>
     </row>
-    <row r="157" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>284</v>
       </c>
@@ -12719,7 +12719,7 @@
         <v>28516055.182341602</v>
       </c>
     </row>
-    <row r="158" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>284</v>
       </c>
@@ -12788,7 +12788,7 @@
         <v>32903140.595009599</v>
       </c>
     </row>
-    <row r="159" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>284</v>
       </c>
@@ -12857,7 +12857,7 @@
         <v>15668162.1880998</v>
       </c>
     </row>
-    <row r="160" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>284</v>
       </c>
@@ -12926,7 +12926,7 @@
         <v>7000000</v>
       </c>
     </row>
-    <row r="161" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>284</v>
       </c>
@@ -12995,7 +12995,7 @@
         <v>7000000</v>
       </c>
     </row>
-    <row r="162" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>284</v>
       </c>
@@ -13064,7 +13064,7 @@
         <v>7000000</v>
       </c>
     </row>
-    <row r="163" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>284</v>
       </c>
@@ -13133,7 +13133,7 @@
         <v>7000000</v>
       </c>
     </row>
-    <row r="164" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>284</v>
       </c>
@@ -13202,7 +13202,7 @@
         <v>7000000</v>
       </c>
     </row>
-    <row r="165" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>284</v>
       </c>
@@ -13271,7 +13271,7 @@
         <v>7000000</v>
       </c>
     </row>
-    <row r="166" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>284</v>
       </c>
@@ -13340,7 +13340,7 @@
         <v>7000000</v>
       </c>
     </row>
-    <row r="167" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>284</v>
       </c>
@@ -13409,7 +13409,7 @@
         <v>7000000</v>
       </c>
     </row>
-    <row r="168" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>300</v>
       </c>
@@ -13478,7 +13478,7 @@
         <v>855.18234165067202</v>
       </c>
     </row>
-    <row r="169" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>301</v>
       </c>
@@ -13547,7 +13547,7 @@
         <v>249867.68969289801</v>
       </c>
     </row>
-    <row r="170" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>301</v>
       </c>
@@ -13616,7 +13616,7 @@
         <v>237736.317332053</v>
       </c>
     </row>
-    <row r="171" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>303</v>
       </c>
@@ -13685,7 +13685,7 @@
         <v>551434.03512476</v>
       </c>
     </row>
-    <row r="172" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>303</v>
       </c>
@@ -13754,7 +13754,7 @@
         <v>801574.87005758099</v>
       </c>
     </row>
-    <row r="173" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>304</v>
       </c>
@@ -13823,7 +13823,7 @@
         <v>168666.39155470199</v>
       </c>
     </row>
-    <row r="174" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>304</v>
       </c>
@@ -13892,7 +13892,7 @@
         <v>190167.87466410699</v>
       </c>
     </row>
-    <row r="175" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>304</v>
       </c>
@@ -13961,7 +13961,7 @@
         <v>132831.80806141999</v>
       </c>
     </row>
-    <row r="176" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>305</v>
       </c>
@@ -14030,7 +14030,7 @@
         <v>639537.11900191905</v>
       </c>
     </row>
-    <row r="177" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>305</v>
       </c>
@@ -14099,7 +14099,7 @@
         <v>705019.40825335903</v>
       </c>
     </row>
-    <row r="178" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>305</v>
       </c>
@@ -14168,7 +14168,7 @@
         <v>530401.19193857897</v>
       </c>
     </row>
-    <row r="179" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>306</v>
       </c>
@@ -14237,7 +14237,7 @@
         <v>43434.711132437602</v>
       </c>
     </row>
-    <row r="180" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>306</v>
       </c>
@@ -14306,7 +14306,7 @@
         <v>44656.400191938497</v>
       </c>
     </row>
-    <row r="181" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>307</v>
       </c>
@@ -14375,7 +14375,7 @@
         <v>525240.77735124703</v>
       </c>
     </row>
-    <row r="182" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>307</v>
       </c>
@@ -14444,7 +14444,7 @@
         <v>530127.53358925099</v>
       </c>
     </row>
-    <row r="183" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>308</v>
       </c>
@@ -14513,7 +14513,7 @@
         <v>184604.54702495199</v>
       </c>
     </row>
-    <row r="184" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>309</v>
       </c>
@@ -14582,7 +14582,7 @@
         <v>916181.27639155404</v>
       </c>
     </row>
-    <row r="185" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>310</v>
       </c>
@@ -14651,7 +14651,7 @@
         <v>184604.54702495199</v>
       </c>
     </row>
-    <row r="186" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>311</v>
       </c>
@@ -14720,7 +14720,7 @@
         <v>916181.27639155404</v>
       </c>
     </row>
-    <row r="187" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>312</v>
       </c>
@@ -14789,7 +14789,7 @@
         <v>1561.9172456813801</v>
       </c>
     </row>
-    <row r="188" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>313</v>
       </c>
@@ -14858,7 +14858,7 @@
         <v>5215.8792706333898</v>
       </c>
     </row>
-    <row r="189" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>314</v>
       </c>
@@ -14927,7 +14927,7 @@
         <v>21674.730834932801</v>
       </c>
     </row>
-    <row r="190" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>315</v>
       </c>
@@ -14996,7 +14996,7 @@
         <v>41104.436986564302</v>
       </c>
     </row>
-    <row r="191" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>316</v>
       </c>
@@ -15065,7 +15065,7 @@
         <v>185657.23983685201</v>
       </c>
     </row>
-    <row r="192" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>317</v>
       </c>
@@ -15134,7 +15134,7 @@
         <v>586905.37380998</v>
       </c>
     </row>
-    <row r="193" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>318</v>
       </c>
@@ -15203,7 +15203,7 @@
         <v>30173365.354952</v>
       </c>
     </row>
-    <row r="194" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>322</v>
       </c>
@@ -15272,7 +15272,7 @@
         <v>37786955.115710102</v>
       </c>
     </row>
-    <row r="195" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>325</v>
       </c>
@@ -15341,7 +15341,7 @@
         <v>35057302.545451</v>
       </c>
     </row>
-    <row r="196" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>325</v>
       </c>
@@ -15410,7 +15410,7 @@
         <v>62042707.548934698</v>
       </c>
     </row>
-    <row r="197" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>329</v>
       </c>
@@ -15479,7 +15479,7 @@
         <v>35057302.545451</v>
       </c>
     </row>
-    <row r="198" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>331</v>
       </c>
@@ -15548,7 +15548,7 @@
         <v>25629069.585595001</v>
       </c>
     </row>
-    <row r="199" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>331</v>
       </c>
@@ -15617,7 +15617,7 @@
         <v>25629069.585595001</v>
       </c>
     </row>
-    <row r="200" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>331</v>
       </c>
@@ -15686,7 +15686,7 @@
         <v>3843181.8200383801</v>
       </c>
     </row>
-    <row r="201" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>331</v>
       </c>
@@ -15755,7 +15755,7 @@
         <v>25629069.585595001</v>
       </c>
     </row>
-    <row r="202" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>331</v>
       </c>
@@ -15824,7 +15824,7 @@
         <v>25629069.585595001</v>
       </c>
     </row>
-    <row r="203" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>331</v>
       </c>
@@ -15893,7 +15893,7 @@
         <v>3843181.8200383801</v>
       </c>
     </row>
-    <row r="204" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>339</v>
       </c>
@@ -15962,7 +15962,7 @@
         <v>206948172.77783099</v>
       </c>
     </row>
-    <row r="205" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>342</v>
       </c>
@@ -16031,7 +16031,7 @@
         <v>15668162.1880998</v>
       </c>
     </row>
-    <row r="206" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>343</v>
       </c>
@@ -16100,7 +16100,7 @@
         <v>855.18234165067202</v>
       </c>
     </row>
-    <row r="207" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>344</v>
       </c>
@@ -16169,7 +16169,7 @@
         <v>187400.77337811899</v>
       </c>
     </row>
-    <row r="208" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>344</v>
       </c>
@@ -16238,7 +16238,7 @@
         <v>187400.77337811899</v>
       </c>
     </row>
-    <row r="209" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>344</v>
       </c>
@@ -16307,7 +16307,7 @@
         <v>178302.24410748499</v>
       </c>
     </row>
-    <row r="210" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>345</v>
       </c>
@@ -16376,7 +16376,7 @@
         <v>413575.52634356997</v>
       </c>
     </row>
-    <row r="211" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>345</v>
       </c>
@@ -16445,7 +16445,7 @@
         <v>601181.15254318598</v>
       </c>
     </row>
-    <row r="212" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>346</v>
       </c>
@@ -16514,7 +16514,7 @@
         <v>126499.793666026</v>
       </c>
     </row>
-    <row r="213" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>346</v>
       </c>
@@ -16583,7 +16583,7 @@
         <v>142625.90599808001</v>
       </c>
     </row>
-    <row r="214" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>346</v>
       </c>
@@ -16652,7 +16652,7 @@
         <v>99623.856046065193</v>
       </c>
     </row>
-    <row r="215" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>347</v>
       </c>
@@ -16721,7 +16721,7 @@
         <v>479652.83925143903</v>
       </c>
     </row>
-    <row r="216" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>347</v>
       </c>
@@ -16790,7 +16790,7 @@
         <v>528764.55619001901</v>
       </c>
     </row>
-    <row r="217" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>347</v>
       </c>
@@ -16859,7 +16859,7 @@
         <v>397800.89395393402</v>
       </c>
     </row>
-    <row r="218" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>348</v>
       </c>
@@ -16928,7 +16928,7 @@
         <v>65152.066698656403</v>
       </c>
     </row>
-    <row r="219" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>348</v>
       </c>
@@ -16997,7 +16997,7 @@
         <v>66984.600287907801</v>
       </c>
     </row>
-    <row r="220" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>349</v>
       </c>
@@ -17066,7 +17066,7 @@
         <v>393930.58301343501</v>
       </c>
     </row>
-    <row r="221" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>349</v>
       </c>
@@ -17135,7 +17135,7 @@
         <v>397595.65019193798</v>
       </c>
     </row>
-    <row r="222" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>350</v>
       </c>
@@ -17204,7 +17204,7 @@
         <v>138453.41026871401</v>
       </c>
     </row>
-    <row r="223" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>351</v>
       </c>
@@ -17273,7 +17273,7 @@
         <v>687135.95729366597</v>
       </c>
     </row>
-    <row r="224" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>352</v>
       </c>
@@ -17342,7 +17342,7 @@
         <v>138453.41026871401</v>
       </c>
     </row>
-    <row r="225" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>353</v>
       </c>
@@ -17411,7 +17411,7 @@
         <v>687135.95729366597</v>
       </c>
     </row>
-    <row r="226" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>354</v>
       </c>
@@ -17480,7 +17480,7 @@
         <v>-325639.77721689001</v>
       </c>
     </row>
-    <row r="227" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>354</v>
       </c>
@@ -17549,7 +17549,7 @@
         <v>-36224790.978886701</v>
       </c>
     </row>
-    <row r="228" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>354</v>
       </c>
@@ -17618,7 +17618,7 @@
         <v>15668162.1880998</v>
       </c>
     </row>
-    <row r="229" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>358</v>
       </c>
@@ -17687,7 +17687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>358</v>
       </c>
@@ -17756,7 +17756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>358</v>
       </c>
@@ -17825,7 +17825,7 @@
         <v>-12000000</v>
       </c>
     </row>
-    <row r="232" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>358</v>
       </c>
@@ -17894,7 +17894,7 @@
         <v>-12000000</v>
       </c>
     </row>
-    <row r="233" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>358</v>
       </c>
@@ -17963,7 +17963,7 @@
         <v>12000000</v>
       </c>
     </row>
-    <row r="234" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>358</v>
       </c>
@@ -18032,7 +18032,7 @@
         <v>12000000</v>
       </c>
     </row>
-    <row r="235" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>366</v>
       </c>
@@ -18101,7 +18101,7 @@
         <v>855.18234165067202</v>
       </c>
     </row>
-    <row r="236" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>367</v>
       </c>
@@ -18170,7 +18170,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="237" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>370</v>
       </c>
@@ -18239,7 +18239,7 @@
         <v>12.216890599999999</v>
       </c>
     </row>
-    <row r="238" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>374</v>
       </c>
@@ -18308,7 +18308,7 @@
         <v>24.433781190000001</v>
       </c>
     </row>
-    <row r="239" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>377</v>
       </c>
@@ -18377,7 +18377,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="240" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>380</v>
       </c>
@@ -18446,7 +18446,7 @@
         <v>366.50671790000001</v>
       </c>
     </row>
-    <row r="241" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>380</v>
       </c>
@@ -18515,7 +18515,7 @@
         <v>488.67562379999998</v>
       </c>
     </row>
-    <row r="242" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>384</v>
       </c>
@@ -18587,7 +18587,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="243" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>384</v>
       </c>
@@ -18659,7 +18659,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="244" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>384</v>
       </c>
@@ -18731,7 +18731,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="245" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>384</v>
       </c>
@@ -18803,7 +18803,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="246" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>384</v>
       </c>
@@ -18875,7 +18875,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="247" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>384</v>
       </c>
@@ -18947,7 +18947,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="248" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>398</v>
       </c>
@@ -19019,7 +19019,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="249" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>398</v>
       </c>
@@ -19091,7 +19091,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="250" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>398</v>
       </c>
@@ -19163,7 +19163,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="251" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>398</v>
       </c>
@@ -19235,7 +19235,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="252" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>398</v>
       </c>
@@ -19307,7 +19307,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="253" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>398</v>
       </c>
@@ -19379,7 +19379,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="254" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>399</v>
       </c>
@@ -19451,7 +19451,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="255" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>399</v>
       </c>
@@ -19523,7 +19523,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="256" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>399</v>
       </c>
@@ -19595,7 +19595,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="257" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>399</v>
       </c>
@@ -19667,7 +19667,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="258" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>399</v>
       </c>
@@ -19739,7 +19739,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="259" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>399</v>
       </c>
@@ -19811,7 +19811,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="260" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>400</v>
       </c>
@@ -19883,7 +19883,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="261" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>400</v>
       </c>
@@ -19955,7 +19955,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="262" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>400</v>
       </c>
@@ -20027,7 +20027,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="263" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>400</v>
       </c>
@@ -20099,7 +20099,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="264" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>400</v>
       </c>
@@ -20171,7 +20171,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="265" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>400</v>
       </c>
@@ -20243,7 +20243,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="266" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>400</v>
       </c>
@@ -20315,7 +20315,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="267" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>403</v>
       </c>
@@ -20387,7 +20387,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="268" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>403</v>
       </c>
@@ -20459,7 +20459,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="269" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>403</v>
       </c>
@@ -20531,7 +20531,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="270" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>403</v>
       </c>
@@ -20603,7 +20603,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="271" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>403</v>
       </c>
@@ -20675,7 +20675,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="272" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>403</v>
       </c>
@@ -20747,7 +20747,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="273" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>403</v>
       </c>
@@ -20819,7 +20819,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="274" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>404</v>
       </c>
@@ -20891,7 +20891,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="275" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>404</v>
       </c>
@@ -20963,7 +20963,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="276" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>404</v>
       </c>
@@ -21035,7 +21035,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="277" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>404</v>
       </c>
@@ -21107,7 +21107,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="278" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>404</v>
       </c>
@@ -21179,7 +21179,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="279" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>404</v>
       </c>
@@ -21251,7 +21251,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="280" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>404</v>
       </c>
@@ -21323,7 +21323,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="281" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>405</v>
       </c>
@@ -21395,7 +21395,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="282" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>405</v>
       </c>
@@ -21467,7 +21467,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="283" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>405</v>
       </c>
@@ -21539,7 +21539,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="284" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>405</v>
       </c>
@@ -21611,7 +21611,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="285" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>405</v>
       </c>
@@ -21683,7 +21683,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="286" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>405</v>
       </c>
@@ -21755,7 +21755,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="287" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>406</v>
       </c>
@@ -21827,7 +21827,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="288" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>406</v>
       </c>
@@ -21899,7 +21899,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="289" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>406</v>
       </c>
@@ -21971,7 +21971,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="290" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>406</v>
       </c>
@@ -22043,7 +22043,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="291" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>406</v>
       </c>
@@ -22115,7 +22115,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="292" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>406</v>
       </c>
@@ -22187,7 +22187,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="293" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>407</v>
       </c>
@@ -22259,7 +22259,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="294" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>407</v>
       </c>
@@ -22331,7 +22331,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="295" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>407</v>
       </c>
@@ -22403,7 +22403,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="296" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>407</v>
       </c>
@@ -22475,7 +22475,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="297" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>407</v>
       </c>
@@ -22547,7 +22547,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="298" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>407</v>
       </c>
@@ -22619,7 +22619,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="299" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>408</v>
       </c>
@@ -22691,7 +22691,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="300" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>408</v>
       </c>
@@ -22763,7 +22763,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="301" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>408</v>
       </c>
@@ -22835,7 +22835,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="302" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>408</v>
       </c>
@@ -22907,7 +22907,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="303" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>408</v>
       </c>
@@ -22979,7 +22979,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="304" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>408</v>
       </c>
@@ -23051,7 +23051,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="305" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>408</v>
       </c>
@@ -23123,7 +23123,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="306" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>409</v>
       </c>
@@ -23195,7 +23195,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="307" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>409</v>
       </c>
@@ -23267,7 +23267,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="308" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>409</v>
       </c>
@@ -23339,7 +23339,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="309" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>409</v>
       </c>
@@ -23411,7 +23411,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="310" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>409</v>
       </c>
@@ -23483,7 +23483,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="311" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>409</v>
       </c>
@@ -23555,7 +23555,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="312" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>409</v>
       </c>
@@ -23627,7 +23627,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="313" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>410</v>
       </c>
@@ -23699,7 +23699,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="314" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>410</v>
       </c>
@@ -23771,7 +23771,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="315" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>410</v>
       </c>
@@ -23843,7 +23843,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="316" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>410</v>
       </c>
@@ -23915,7 +23915,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="317" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>410</v>
       </c>
@@ -23987,7 +23987,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="318" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>410</v>
       </c>
@@ -24059,7 +24059,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="319" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>410</v>
       </c>
@@ -24131,7 +24131,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="320" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>411</v>
       </c>
@@ -24203,7 +24203,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="321" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>411</v>
       </c>
@@ -24275,7 +24275,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="322" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>411</v>
       </c>
@@ -24347,7 +24347,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="323" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>411</v>
       </c>
@@ -24419,7 +24419,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="324" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>411</v>
       </c>
@@ -24491,7 +24491,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="325" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>411</v>
       </c>
@@ -24563,7 +24563,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="326" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>419</v>
       </c>
@@ -24635,7 +24635,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="327" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>419</v>
       </c>
@@ -24707,7 +24707,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="328" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>419</v>
       </c>
@@ -24779,7 +24779,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="329" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>419</v>
       </c>
@@ -24851,7 +24851,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="330" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>421</v>
       </c>
@@ -24920,7 +24920,7 @@
         <v>183.25335889999999</v>
       </c>
     </row>
-    <row r="331" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>421</v>
       </c>
@@ -24989,7 +24989,7 @@
         <v>305.42226490000002</v>
       </c>
     </row>
-    <row r="332" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>426</v>
       </c>
@@ -25058,7 +25058,7 @@
         <v>305.42226490000002</v>
       </c>
     </row>
-    <row r="333" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>428</v>
       </c>
@@ -25127,7 +25127,7 @@
         <v>305.42226490000002</v>
       </c>
     </row>
-    <row r="334" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>430</v>
       </c>
@@ -25196,7 +25196,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="335" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>432</v>
       </c>
@@ -25265,7 +25265,7 @@
         <v>-35</v>
       </c>
     </row>
-    <row r="336" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>432</v>
       </c>
@@ -25334,7 +25334,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="337" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>432</v>
       </c>
@@ -25403,7 +25403,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="338" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>432</v>
       </c>
@@ -25472,7 +25472,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="339" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>432</v>
       </c>
@@ -25541,7 +25541,7 @@
         <v>-40</v>
       </c>
     </row>
-    <row r="340" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>439</v>
       </c>
@@ -25610,7 +25610,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="341" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>439</v>
       </c>
@@ -25679,7 +25679,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="342" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>439</v>
       </c>
@@ -25748,7 +25748,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="343" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>439</v>
       </c>
@@ -25817,7 +25817,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="344" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>439</v>
       </c>
@@ -25886,7 +25886,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="345" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>439</v>
       </c>
@@ -25955,7 +25955,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="346" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>439</v>
       </c>
@@ -26024,7 +26024,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="347" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>439</v>
       </c>
@@ -26093,7 +26093,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="348" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>439</v>
       </c>
@@ -26162,7 +26162,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="349" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>439</v>
       </c>
@@ -26231,7 +26231,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="350" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>439</v>
       </c>
@@ -26300,7 +26300,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="351" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>450</v>
       </c>
@@ -26369,7 +26369,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="352" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>450</v>
       </c>
@@ -26438,7 +26438,7 @@
         <v>25000000</v>
       </c>
     </row>
-    <row r="353" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>450</v>
       </c>
@@ -26507,7 +26507,7 @@
         <v>25000000</v>
       </c>
     </row>
-    <row r="354" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>456</v>
       </c>
@@ -26576,7 +26576,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="355" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>456</v>
       </c>
@@ -26645,7 +26645,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="356" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>460</v>
       </c>
@@ -26714,7 +26714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="357" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>460</v>
       </c>
@@ -26783,7 +26783,7 @@
         <v>-4700</v>
       </c>
     </row>
-    <row r="358" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>460</v>
       </c>
@@ -26852,7 +26852,7 @@
         <v>-3000</v>
       </c>
     </row>
-    <row r="359" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>460</v>
       </c>
@@ -26921,7 +26921,7 @@
         <v>-8900</v>
       </c>
     </row>
-    <row r="360" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>466</v>
       </c>
@@ -26990,7 +26990,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="361" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>466</v>
       </c>
@@ -27059,7 +27059,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="362" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>466</v>
       </c>
@@ -27128,7 +27128,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="363" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>466</v>
       </c>
@@ -27197,7 +27197,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="364" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>466</v>
       </c>
@@ -27266,7 +27266,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="365" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>466</v>
       </c>
@@ -27335,7 +27335,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="366" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>474</v>
       </c>
@@ -27404,7 +27404,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="367" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>474</v>
       </c>
@@ -27473,7 +27473,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="368" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>474</v>
       </c>
@@ -27542,7 +27542,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="369" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>479</v>
       </c>
@@ -27611,7 +27611,7 @@
         <v>23000</v>
       </c>
     </row>
-    <row r="370" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>479</v>
       </c>
@@ -27680,7 +27680,7 @@
         <v>23000</v>
       </c>
     </row>
-    <row r="371" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>479</v>
       </c>
@@ -27749,7 +27749,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="372" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>484</v>
       </c>
@@ -27818,7 +27818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="373" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>484</v>
       </c>
@@ -27887,7 +27887,7 @@
         <v>6300</v>
       </c>
     </row>
-    <row r="374" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>484</v>
       </c>
@@ -27956,7 +27956,7 @@
         <v>6300</v>
       </c>
     </row>
-    <row r="375" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>484</v>
       </c>
@@ -28025,7 +28025,7 @@
         <v>6300</v>
       </c>
     </row>
-    <row r="376" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>490</v>
       </c>
@@ -28094,7 +28094,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="377" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>493</v>
       </c>
@@ -28163,7 +28163,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="378" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>495</v>
       </c>
@@ -28222,7 +28222,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="379" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>495</v>
       </c>
@@ -28281,7 +28281,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="380" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>499</v>
       </c>
@@ -28340,7 +28340,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="381" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>499</v>
       </c>
@@ -28399,7 +28399,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="382" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>502</v>
       </c>
@@ -28458,7 +28458,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="383" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>502</v>
       </c>
@@ -28517,7 +28517,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="384" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>504</v>
       </c>
@@ -28586,7 +28586,7 @@
         <v>-1404201.01198656</v>
       </c>
     </row>
-    <row r="385" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>504</v>
       </c>
@@ -28655,7 +28655,7 @@
         <v>-1474411.0668617999</v>
       </c>
     </row>
-    <row r="386" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>508</v>
       </c>

</xml_diff>